<commit_message>
update the miRNA_analysis_for_neuronClassess.R and miRNAseq_functions.R with the expressed and mature miRNAs part
</commit_message>
<xml_diff>
--- a/exp_design/Neuron_project_design_all_v1.xlsx
+++ b/exp_design/Neuron_project_design_all_v1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/groups/cochella/jiwang/Projects/Chiara/Project_neuronal_miRNAs/exp_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453B60AF-9BD3-DD41-B3DB-D1AADC5C74BA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41680" yWindow="-12120" windowWidth="36780" windowHeight="30040" tabRatio="500"/>
+    <workbookView xWindow="35640" yWindow="-12380" windowWidth="42300" windowHeight="30040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$53</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="132">
   <si>
     <t xml:space="preserve">Library </t>
   </si>
@@ -396,12 +397,42 @@
   </si>
   <si>
     <t>unc-42 expressing neurons</t>
+  </si>
+  <si>
+    <t>L3 WT Treatment (N2), technical replicate #1 (no spikeIns)</t>
+  </si>
+  <si>
+    <t>L3 WT No treatment (N2), technical replicate #1 (no spikeIns)</t>
+  </si>
+  <si>
+    <t>L3 WT Treatment (N2), technical replicate #2(no spikeIns)</t>
+  </si>
+  <si>
+    <t>L3 WT No treatment (N2), technical replicate #2(no spikeIns)</t>
+  </si>
+  <si>
+    <t>L3 OS11358 Treatment(no spikeIns)</t>
+  </si>
+  <si>
+    <t>L3 OS11358 No treatment(no spikeIns)</t>
+  </si>
+  <si>
+    <t>L3 OS11359 Treatment(no spikeIns)</t>
+  </si>
+  <si>
+    <t>L3 OS11359 No treatment(no spikeIns)</t>
+  </si>
+  <si>
+    <t>whole.body.L3</t>
+  </si>
+  <si>
+    <t>CEPsh.L3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -540,6 +571,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -807,14 +841,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80:F83"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,7 +857,7 @@
     <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="49.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52" style="1" customWidth="1"/>
     <col min="6" max="6" width="50.1640625" style="1" customWidth="1"/>
     <col min="7" max="8" width="55.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="50.1640625" style="1" customWidth="1"/>
@@ -3237,6 +3271,238 @@
         <v>116</v>
       </c>
     </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="5">
+        <v>43243</v>
+      </c>
+      <c r="B85" s="1">
+        <v>6239</v>
+      </c>
+      <c r="C85" s="1">
+        <v>6165</v>
+      </c>
+      <c r="D85" s="1">
+        <v>66867</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="5">
+        <v>43243</v>
+      </c>
+      <c r="B86" s="1">
+        <v>6239</v>
+      </c>
+      <c r="C86" s="1">
+        <v>6165</v>
+      </c>
+      <c r="D86" s="1">
+        <v>66868</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="5">
+        <v>43243</v>
+      </c>
+      <c r="B87" s="1">
+        <v>6239</v>
+      </c>
+      <c r="C87" s="1">
+        <v>6165</v>
+      </c>
+      <c r="D87" s="1">
+        <v>66869</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
+        <v>43243</v>
+      </c>
+      <c r="B88" s="1">
+        <v>6239</v>
+      </c>
+      <c r="C88" s="1">
+        <v>6165</v>
+      </c>
+      <c r="D88" s="1">
+        <v>66870</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="5">
+        <v>43243</v>
+      </c>
+      <c r="B89" s="1">
+        <v>6239</v>
+      </c>
+      <c r="C89" s="1">
+        <v>6165</v>
+      </c>
+      <c r="D89" s="1">
+        <v>66871</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
+        <v>43243</v>
+      </c>
+      <c r="B90" s="1">
+        <v>6239</v>
+      </c>
+      <c r="C90" s="1">
+        <v>6165</v>
+      </c>
+      <c r="D90" s="1">
+        <v>66872</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>43243</v>
+      </c>
+      <c r="B91" s="1">
+        <v>6239</v>
+      </c>
+      <c r="C91" s="1">
+        <v>6165</v>
+      </c>
+      <c r="D91" s="1">
+        <v>66873</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
+        <v>43243</v>
+      </c>
+      <c r="B92" s="1">
+        <v>6239</v>
+      </c>
+      <c r="C92" s="1">
+        <v>6165</v>
+      </c>
+      <c r="D92" s="1">
+        <v>66874</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update design matrxi by addign rab-3 WT and update the scripts/prepare_ExpressionMatrix.R by adding rab-3 WT
</commit_message>
<xml_diff>
--- a/exp_design/Neuron_project_design_all_v1.xlsx
+++ b/exp_design/Neuron_project_design_all_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/groups/cochella/jiwang/Projects/Chiara/Project_neuronal_miRNAs/exp_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453B60AF-9BD3-DD41-B3DB-D1AADC5C74BA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E65C38-9B88-D849-B9E9-B4DE1CDDDA3D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35640" yWindow="-12380" windowWidth="42300" windowHeight="30040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33320" yWindow="-12920" windowWidth="42300" windowHeight="30040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="137">
   <si>
     <t xml:space="preserve">Library </t>
   </si>
@@ -427,6 +427,21 @@
   </si>
   <si>
     <t>CEPsh.L3</t>
+  </si>
+  <si>
+    <t>WT, spike-ins added</t>
+  </si>
+  <si>
+    <t>rab-3:HEN1 MLC416 No Treatment L1 (prep 9) WT, spike-ins added</t>
+  </si>
+  <si>
+    <t>rab-3:HEN1 MLC416 Treatment L1 (prep 9) WT, spike-ins added</t>
+  </si>
+  <si>
+    <t>rab-3:HEN1 MLC417 No Treatment L1 (prep 6) WT, spike-ins added</t>
+  </si>
+  <si>
+    <t>rab-3:HEN1 MLC417 Treatment L1 (prep 6) WT, spike-ins added</t>
   </si>
 </sst>
 </file>
@@ -515,7 +530,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -539,6 +554,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -845,10 +866,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3503,6 +3524,122 @@
         <v>129</v>
       </c>
     </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="9">
+        <v>43320</v>
+      </c>
+      <c r="B93" s="10">
+        <v>6585</v>
+      </c>
+      <c r="C93" s="10">
+        <v>6596</v>
+      </c>
+      <c r="D93" s="10">
+        <v>71820</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H93" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="9">
+        <v>43320</v>
+      </c>
+      <c r="B94" s="10">
+        <v>6585</v>
+      </c>
+      <c r="C94" s="10">
+        <v>6596</v>
+      </c>
+      <c r="D94" s="10">
+        <v>71821</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="9">
+        <v>43320</v>
+      </c>
+      <c r="B95" s="10">
+        <v>6585</v>
+      </c>
+      <c r="C95" s="10">
+        <v>6596</v>
+      </c>
+      <c r="D95" s="10">
+        <v>71822</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H95" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="9">
+        <v>43320</v>
+      </c>
+      <c r="B96" s="10">
+        <v>6585</v>
+      </c>
+      <c r="C96" s="10">
+        <v>6596</v>
+      </c>
+      <c r="D96" s="10">
+        <v>71823</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update the exp_design file with unc-3, which is the last sample in this project
</commit_message>
<xml_diff>
--- a/exp_design/Neuron_project_design_all_v1.xlsx
+++ b/exp_design/Neuron_project_design_all_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/groups/cochella/jiwang/Projects/Chiara/Project_neuronal_miRNAs/exp_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E65C38-9B88-D849-B9E9-B4DE1CDDDA3D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96055EE1-098F-5E4C-AAE4-581E614B6040}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33320" yWindow="-12920" windowWidth="42300" windowHeight="30040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33320" yWindow="-12920" windowWidth="44320" windowHeight="30300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="144">
   <si>
     <t xml:space="preserve">Library </t>
   </si>
@@ -442,6 +442,27 @@
   </si>
   <si>
     <t>rab-3:HEN1 MLC417 Treatment L1 (prep 6) WT, spike-ins added</t>
+  </si>
+  <si>
+    <t>MLC1602 unc-3:Ath-HEN1 L1s -A, prep1- No treatment</t>
+  </si>
+  <si>
+    <t>MLC1602 unc-3:Ath-HEN1 L1s -A, prep1- Treatment</t>
+  </si>
+  <si>
+    <t>MLC1602 unc-3:Ath-HEN1 L1s -B, prep1- No treatment</t>
+  </si>
+  <si>
+    <t>MLC1602 unc-3:Ath-HEN1 L1s -B, prep1- Treatment</t>
+  </si>
+  <si>
+    <t>unc-3 expressing neurons</t>
+  </si>
+  <si>
+    <t>unc-3</t>
+  </si>
+  <si>
+    <t>unc-3 is a transcriptional factor</t>
   </si>
 </sst>
 </file>
@@ -866,10 +887,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView tabSelected="1" topLeftCell="E68" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3640,6 +3661,122 @@
         <v>132</v>
       </c>
     </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
+        <v>43322</v>
+      </c>
+      <c r="B97" s="1">
+        <v>6625</v>
+      </c>
+      <c r="C97" s="1">
+        <v>6641</v>
+      </c>
+      <c r="D97" s="1">
+        <v>72762</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>43322</v>
+      </c>
+      <c r="B98" s="1">
+        <v>6625</v>
+      </c>
+      <c r="C98" s="1">
+        <v>6641</v>
+      </c>
+      <c r="D98" s="1">
+        <v>72763</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>43322</v>
+      </c>
+      <c r="B99" s="1">
+        <v>6625</v>
+      </c>
+      <c r="C99" s="1">
+        <v>6641</v>
+      </c>
+      <c r="D99" s="1">
+        <v>72764</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
+        <v>43322</v>
+      </c>
+      <c r="B100" s="1">
+        <v>6625</v>
+      </c>
+      <c r="C100" s="1">
+        <v>6641</v>
+      </c>
+      <c r="D100" s="1">
+        <v>72765</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update and backup for new rab-3 and rgef-1 pan-neurons
</commit_message>
<xml_diff>
--- a/exp_design/Neuron_project_design_all_v1.xlsx
+++ b/exp_design/Neuron_project_design_all_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/groups/cochella/jiwang/Projects/Chiara/Project_neuronal_miRNAs/exp_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96055EE1-098F-5E4C-AAE4-581E614B6040}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B774CD45-8563-2D44-92C7-FB42BA244775}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33320" yWindow="-12920" windowWidth="44320" windowHeight="30300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="160">
   <si>
     <t xml:space="preserve">Library </t>
   </si>
@@ -463,13 +463,61 @@
   </si>
   <si>
     <t>unc-3 is a transcriptional factor</t>
+  </si>
+  <si>
+    <t>MLC532 rgef-1::Ath-HEN1 prep 1, No treatment, + spike-ins</t>
+  </si>
+  <si>
+    <t>Pan-neuronal (all neurons) - L1</t>
+  </si>
+  <si>
+    <t>MLC532 rgef-1::Ath-HEN1 prep 1, Treatment, + spike-ins</t>
+  </si>
+  <si>
+    <t>MLC534 rgef-1::Ath-HEN1 prep 1, No treatment, + spike-ins</t>
+  </si>
+  <si>
+    <t>MLC534 rgef-1::Ath-HEN1 prep 1, Treatment, + spike-ins</t>
+  </si>
+  <si>
+    <t>MLC417 rab-3::Ath-HEN1 prep 1, No treatment, + spike-ins</t>
+  </si>
+  <si>
+    <t>MLC417 rab-3::Ath-HEN1 prep 1, Treatment, + spike-ins</t>
+  </si>
+  <si>
+    <t>MLC416 rab-3::Ath-HEN1 prep 2, No treatment, + spike-ins</t>
+  </si>
+  <si>
+    <t>MLC416 rab-3::Ath-HEN1 prep 2, Treatment, + spike-ins</t>
+  </si>
+  <si>
+    <t>Pan-neuronal (all neurons) - L2</t>
+  </si>
+  <si>
+    <t>Pan-neuronal (all neurons) - L3</t>
+  </si>
+  <si>
+    <t>Pan-neuronal (all neurons) - L4</t>
+  </si>
+  <si>
+    <t>Pan-neuronal (all neurons) - L5</t>
+  </si>
+  <si>
+    <t>Pan-neuronal (all neurons) - L6</t>
+  </si>
+  <si>
+    <t>Pan-neuronal (all neurons) - L7</t>
+  </si>
+  <si>
+    <t>Pan-neuronal (all neurons) - L8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -514,6 +562,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -551,7 +606,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -581,6 +636,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -887,10 +945,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E68" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3546,235 +3605,478 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="9">
+      <c r="A93" s="2">
+        <v>43322</v>
+      </c>
+      <c r="B93" s="1">
+        <v>6625</v>
+      </c>
+      <c r="C93" s="1">
+        <v>6641</v>
+      </c>
+      <c r="D93" s="1">
+        <v>72762</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
+        <v>43322</v>
+      </c>
+      <c r="B94" s="1">
+        <v>6625</v>
+      </c>
+      <c r="C94" s="1">
+        <v>6641</v>
+      </c>
+      <c r="D94" s="1">
+        <v>72763</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
+        <v>43322</v>
+      </c>
+      <c r="B95" s="1">
+        <v>6625</v>
+      </c>
+      <c r="C95" s="1">
+        <v>6641</v>
+      </c>
+      <c r="D95" s="1">
+        <v>72764</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
+        <v>43322</v>
+      </c>
+      <c r="B96" s="1">
+        <v>6625</v>
+      </c>
+      <c r="C96" s="1">
+        <v>6641</v>
+      </c>
+      <c r="D96" s="1">
+        <v>72765</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="9">
         <v>43320</v>
       </c>
-      <c r="B93" s="10">
+      <c r="B98" s="10">
         <v>6585</v>
       </c>
-      <c r="C93" s="10">
+      <c r="C98" s="10">
         <v>6596</v>
       </c>
-      <c r="D93" s="10">
+      <c r="D98" s="10">
         <v>71820</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F93" s="1" t="s">
+      <c r="E98" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F98" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G93" s="4" t="s">
+      <c r="G98" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H93" s="10" t="s">
+      <c r="H98" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="I93" s="1" t="s">
+      <c r="I98" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="9">
         <v>43320</v>
       </c>
-      <c r="B94" s="10">
+      <c r="B99" s="10">
         <v>6585</v>
       </c>
-      <c r="C94" s="10">
+      <c r="C99" s="10">
         <v>6596</v>
       </c>
-      <c r="D94" s="10">
+      <c r="D99" s="10">
         <v>71821</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F94" s="1" t="s">
+      <c r="E99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G94" s="4" t="s">
+      <c r="G99" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H94" s="10" t="s">
+      <c r="H99" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="I94" s="1" t="s">
+      <c r="I99" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" s="9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="9">
         <v>43320</v>
       </c>
-      <c r="B95" s="10">
+      <c r="B100" s="10">
         <v>6585</v>
       </c>
-      <c r="C95" s="10">
+      <c r="C100" s="10">
         <v>6596</v>
       </c>
-      <c r="D95" s="10">
+      <c r="D100" s="10">
         <v>71822</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F95" s="1" t="s">
+      <c r="E100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G95" s="4" t="s">
+      <c r="G100" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H95" s="10" t="s">
+      <c r="H100" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="I95" s="1" t="s">
+      <c r="I100" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="9">
         <v>43320</v>
       </c>
-      <c r="B96" s="10">
+      <c r="B101" s="10">
         <v>6585</v>
       </c>
-      <c r="C96" s="10">
+      <c r="C101" s="10">
         <v>6596</v>
       </c>
-      <c r="D96" s="10">
+      <c r="D101" s="10">
         <v>71823</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F96" s="1" t="s">
+      <c r="E101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G96" s="4" t="s">
+      <c r="G101" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H96" s="10" t="s">
+      <c r="H101" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="I96" s="1" t="s">
+      <c r="I101" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="2">
-        <v>43322</v>
-      </c>
-      <c r="B97" s="1">
-        <v>6625</v>
-      </c>
-      <c r="C97" s="1">
-        <v>6641</v>
-      </c>
-      <c r="D97" s="1">
-        <v>72762</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98" s="2">
-        <v>43322</v>
-      </c>
-      <c r="B98" s="1">
-        <v>6625</v>
-      </c>
-      <c r="C98" s="1">
-        <v>6641</v>
-      </c>
-      <c r="D98" s="1">
-        <v>72763</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A99" s="2">
-        <v>43322</v>
-      </c>
-      <c r="B99" s="1">
-        <v>6625</v>
-      </c>
-      <c r="C99" s="1">
-        <v>6641</v>
-      </c>
-      <c r="D99" s="1">
-        <v>72764</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A100" s="2">
-        <v>43322</v>
-      </c>
-      <c r="B100" s="1">
-        <v>6625</v>
-      </c>
-      <c r="C100" s="1">
-        <v>6641</v>
-      </c>
-      <c r="D100" s="1">
-        <v>72765</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>143</v>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" s="9"/>
+      <c r="B102" s="10"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="10"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="10"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
+        <v>43412</v>
+      </c>
+      <c r="B103" s="1">
+        <v>7011</v>
+      </c>
+      <c r="C103" s="1">
+        <v>7088</v>
+      </c>
+      <c r="D103" s="11">
+        <v>78316</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H103" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
+        <v>43412</v>
+      </c>
+      <c r="B104" s="1">
+        <v>7011</v>
+      </c>
+      <c r="C104" s="1">
+        <v>7088</v>
+      </c>
+      <c r="D104" s="11">
+        <v>78317</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H104" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
+        <v>43412</v>
+      </c>
+      <c r="B105" s="1">
+        <v>7011</v>
+      </c>
+      <c r="C105" s="1">
+        <v>7088</v>
+      </c>
+      <c r="D105" s="11">
+        <v>78318</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H105" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
+        <v>43412</v>
+      </c>
+      <c r="B106" s="1">
+        <v>7011</v>
+      </c>
+      <c r="C106" s="1">
+        <v>7088</v>
+      </c>
+      <c r="D106" s="11">
+        <v>78319</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H106" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>43412</v>
+      </c>
+      <c r="B107" s="1">
+        <v>7011</v>
+      </c>
+      <c r="C107" s="1">
+        <v>7088</v>
+      </c>
+      <c r="D107" s="1">
+        <v>78312</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I107" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>43412</v>
+      </c>
+      <c r="B108" s="1">
+        <v>7011</v>
+      </c>
+      <c r="C108" s="1">
+        <v>7088</v>
+      </c>
+      <c r="D108" s="1">
+        <v>78313</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I108" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
+        <v>43412</v>
+      </c>
+      <c r="B109" s="1">
+        <v>7011</v>
+      </c>
+      <c r="C109" s="1">
+        <v>7088</v>
+      </c>
+      <c r="D109" s="11">
+        <v>78314</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I109" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
+        <v>43412</v>
+      </c>
+      <c r="B110" s="1">
+        <v>7011</v>
+      </c>
+      <c r="C110" s="1">
+        <v>7088</v>
+      </c>
+      <c r="D110" s="11">
+        <v>78315</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I110" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
in the middle of analysis for tax4 mutant; still not quite clear how to integrate this analysis into the old ones
</commit_message>
<xml_diff>
--- a/exp_design/Neuron_project_design_all_v1.xlsx
+++ b/exp_design/Neuron_project_design_all_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/groups/cochella/jiwang/Projects/Chiara/Project_neuronal_miRNAs/exp_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B774CD45-8563-2D44-92C7-FB42BA244775}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A93A71D-408E-944F-ABFF-9024FCBC4BBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33320" yWindow="-12920" windowWidth="44320" windowHeight="30300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35680" yWindow="-13060" windowWidth="44320" windowHeight="30300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$53</definedName>
   </definedNames>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="173">
   <si>
     <t xml:space="preserve">Library </t>
   </si>
@@ -511,6 +511,45 @@
   </si>
   <si>
     <t>Pan-neuronal (all neurons) - L8</t>
+  </si>
+  <si>
+    <t>MLC1693 osm-5p::HEN1::unc-54 3’UTR; tax-4 (ks28) No treatment (FA 1:20 dilution)</t>
+  </si>
+  <si>
+    <t>Ciliated neurons that are inactive because mutated in tax-4 channel - L1</t>
+  </si>
+  <si>
+    <t>MLC1693 osm-5p::HEN1::unc-54 3’UTR; tax-4 (ks28) Treatment (FA 1:20 dilution)</t>
+  </si>
+  <si>
+    <t>MLC1694 osm-5p::HEN1::unc-54 3’UTR; tax-4 (ks28) No treatment (FA 1:40 dilution)</t>
+  </si>
+  <si>
+    <t>MLC1694 osm-5p::HEN1::unc-54 3’UTR; tax-4 (ks28) Treatment (FA 1:20 dilution)</t>
+  </si>
+  <si>
+    <t>MLC1695 osm-5p::HEN1::unc-54 3’UTR; tax-4 (p678)III No treatment (FA 1:20 dilution)</t>
+  </si>
+  <si>
+    <t>MLC1695 osm-5p::HEN1::unc-54 3’UTR; tax-4 (p678) Treatment (FA 1:20 dilution)</t>
+  </si>
+  <si>
+    <t>MLC1696 osm-5p::HEN1::unc-54 3’UTR; tax-4 (p678)III No treatment (FA 1:20 dilution)</t>
+  </si>
+  <si>
+    <t>MLC1696 osm-5p::HEN1::unc-54 3’UTR; tax-4 (p678) Treatment (FA 1:20 dilution)</t>
+  </si>
+  <si>
+    <t>MLC1693 osm-5p::HEN1::unc-54 3’UTR; tax-4 (ks28) No treatment (FA 1:40 dilution)</t>
+  </si>
+  <si>
+    <t>WT_tax4_mutant_ks28</t>
+  </si>
+  <si>
+    <t>WT_tax4_mutant_p678</t>
+  </si>
+  <si>
+    <t>osm-5</t>
   </si>
 </sst>
 </file>
@@ -606,7 +645,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -640,6 +679,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -945,11 +987,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,7 +1002,8 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="52" style="1" customWidth="1"/>
     <col min="6" max="6" width="50.1640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="55.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="55.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="92.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="50.1640625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -4079,6 +4122,325 @@
         <v>155</v>
       </c>
     </row>
+    <row r="112" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B112" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C112" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D112" s="1">
+        <v>87655</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H112" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="I112" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B113" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C113" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D113" s="1">
+        <v>87656</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I113" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B114" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C114" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D114" s="11">
+        <v>87657</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I114" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B115" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C115" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D115" s="11">
+        <v>87658</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I115" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B116" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C116" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D116" s="11">
+        <v>87659</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I116" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B117" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C117" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D117" s="11">
+        <v>87660</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I117" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B118" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C118" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D118" s="11">
+        <v>87661</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I118" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B119" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C119" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D119" s="11">
+        <v>87662</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I119" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B120" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C120" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D120" s="11">
+        <v>87663</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H120" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="I120" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B121" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C121" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D121" s="11">
+        <v>87664</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H121" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="I121" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B122" s="1">
+        <v>7794</v>
+      </c>
+      <c r="C122" s="1">
+        <v>8101</v>
+      </c>
+      <c r="D122" s="11">
+        <v>87665</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H122" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="I122" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>